<commit_message>
v1.01, proper support for strings with embedded newline chars
</commit_message>
<xml_diff>
--- a/t/valuereader.xlsx
+++ b/t/valuereader.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" activeTab="3"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Test" sheetId="1" r:id="rId1"/>
@@ -19,13 +19,13 @@
   </sheets>
   <calcPr calcId="162913"/>
   <pivotCaches>
-    <pivotCache cacheId="32" r:id="rId5"/>
+    <pivotCache cacheId="0" r:id="rId5"/>
   </pivotCaches>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="396" uniqueCount="186">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="397" uniqueCount="187">
   <si>
     <t>Hello</t>
   </si>
@@ -606,6 +606,11 @@
   </si>
   <si>
     <t>ampersand</t>
+  </si>
+  <si>
+    <t>cell
+with
+embedded newlines</t>
   </si>
 </sst>
 </file>
@@ -649,7 +654,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -658,6 +663,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1296,7 +1304,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Tableau croisé dynamique2" cacheId="32" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valeurs" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Tableau croisé dynamique2" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valeurs" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:E59" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="6">
     <pivotField showAll="0"/>
@@ -1868,10 +1876,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1926,6 +1934,11 @@
       <c r="F6" t="str">
         <f>A1&amp;" "&amp;B6</f>
         <v>Hello after an empty row and col</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
+        <v>186</v>
       </c>
     </row>
   </sheetData>
@@ -3288,7 +3301,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:E59"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
first attempt to support parsing dates
</commit_message>
<xml_diff>
--- a/t/valuereader.xlsx
+++ b/t/valuereader.xlsx
@@ -9,23 +9,24 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Test" sheetId="1" r:id="rId1"/>
     <sheet name="Empty" sheetId="2" r:id="rId2"/>
     <sheet name="Entities" sheetId="3" r:id="rId3"/>
     <sheet name="Tab_entities" sheetId="5" r:id="rId4"/>
+    <sheet name="Dates" sheetId="6" r:id="rId5"/>
   </sheets>
   <calcPr calcId="162913"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId5"/>
+    <pivotCache cacheId="0" r:id="rId6"/>
   </pivotCaches>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="397" uniqueCount="187">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="399" uniqueCount="189">
   <si>
     <t>Hello</t>
   </si>
@@ -612,12 +613,33 @@
 with
 embedded newlines</t>
   </si>
+  <si>
+    <t>01.02.1789</t>
+  </si>
+  <si>
+    <t>31.12.1899</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <numFmts count="13">
+    <numFmt numFmtId="164" formatCode="dd/mm/yyyy;@"/>
+    <numFmt numFmtId="165" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
+    <numFmt numFmtId="166" formatCode="dd/mm/yyyy\ hh:mm:ss"/>
+    <numFmt numFmtId="167" formatCode="dd/mm/yyyy\ hh:mm:ss.000"/>
+    <numFmt numFmtId="168" formatCode="[h]:mm:ss.000"/>
+    <numFmt numFmtId="169" formatCode="dd/mm/yy;@"/>
+    <numFmt numFmtId="170" formatCode="dd/\ m/\ yy;@"/>
+    <numFmt numFmtId="171" formatCode="d/m/yy;@"/>
+    <numFmt numFmtId="172" formatCode="yyyy\-mm\-dd;@"/>
+    <numFmt numFmtId="173" formatCode="[$-100C]dddd\,\ d/\ mmmm\ yyyy;@"/>
+    <numFmt numFmtId="174" formatCode="[$-100C]d/\ mmmm\ yyyy;@"/>
+    <numFmt numFmtId="175" formatCode="[$-100C]d\ mmm\ yy;@"/>
+    <numFmt numFmtId="176" formatCode="mmm/yyyy"/>
+  </numFmts>
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -627,6 +649,13 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -651,10 +680,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -667,8 +697,27 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="46" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="173" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="174" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="175" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="DateStyleddmmyyyy" xfId="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1878,7 +1927,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
@@ -4157,4 +4206,126 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="23" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.140625" customWidth="1"/>
+    <col min="5" max="5" width="28.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="6">
+        <v>44022</v>
+      </c>
+      <c r="B1" s="7">
+        <v>44022</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>187</v>
+      </c>
+      <c r="D1" s="8">
+        <v>44022.122916666667</v>
+      </c>
+      <c r="E1" s="9">
+        <v>0.12359953703703704</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="10">
+        <v>44022</v>
+      </c>
+      <c r="B2" s="7">
+        <v>44022</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>188</v>
+      </c>
+      <c r="D2" s="11">
+        <v>44022.123599537037</v>
+      </c>
+      <c r="E2" s="12">
+        <v>5.7638888888888885E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="13">
+        <v>44022</v>
+      </c>
+      <c r="C3" s="6">
+        <v>1</v>
+      </c>
+      <c r="D3" s="14"/>
+      <c r="E3" s="15">
+        <v>5.9938888888888889E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="16">
+        <v>44022</v>
+      </c>
+      <c r="C4" s="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="17">
+        <v>44022</v>
+      </c>
+      <c r="C5" s="6">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="18">
+        <v>44022</v>
+      </c>
+      <c r="C6" s="6">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="19">
+        <v>44022</v>
+      </c>
+      <c r="C7" s="6">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="20">
+        <v>44022</v>
+      </c>
+      <c r="C8" s="6">
+        <v>929273</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="21">
+        <v>44022</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="22">
+        <v>44022</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="23">
+        <v>44022</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
testing various date options
</commit_message>
<xml_diff>
--- a/t/valuereader.xlsx
+++ b/t/valuereader.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="399" uniqueCount="189">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="397" uniqueCount="187">
   <si>
     <t>Hello</t>
   </si>
@@ -612,12 +612,6 @@
     <t>cell
 with
 embedded newlines</t>
-  </si>
-  <si>
-    <t>01.02.1789</t>
-  </si>
-  <si>
-    <t>31.12.1899</t>
   </si>
 </sst>
 </file>
@@ -4213,7 +4207,7 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4230,8 +4224,8 @@
       <c r="B1" s="7">
         <v>44022</v>
       </c>
-      <c r="C1" s="6" t="s">
-        <v>187</v>
+      <c r="C1" s="6">
+        <v>32540</v>
       </c>
       <c r="D1" s="8">
         <v>44022.122916666667</v>
@@ -4247,8 +4241,8 @@
       <c r="B2" s="7">
         <v>44022</v>
       </c>
-      <c r="C2" s="6" t="s">
-        <v>188</v>
+      <c r="C2" s="6">
+        <v>36525</v>
       </c>
       <c r="D2" s="11">
         <v>44022.123599537037</v>

</xml_diff>

<commit_message>
v1.05 : suppress warnings when a style is applied to a non-numeric cell
</commit_message>
<xml_diff>
--- a/t/valuereader.xlsx
+++ b/t/valuereader.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" activeTab="4"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Test" sheetId="1" r:id="rId1"/>
@@ -657,12 +657,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -678,7 +684,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -709,6 +715,7 @@
     <xf numFmtId="174" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="175" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="DateStyleddmmyyyy" xfId="1"/>
@@ -1921,8 +1928,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1931,9 +1938,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="24" t="s">
         <v>0</v>
       </c>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
       <c r="D1">
         <v>22</v>
       </c>
@@ -1946,26 +1955,29 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2">
+      <c r="A2" s="24">
         <v>123</v>
       </c>
-      <c r="C2" t="s">
+      <c r="B2" s="24"/>
+      <c r="C2" s="24" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" t="s">
+      <c r="A3" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="24"/>
+      <c r="C3" s="24" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="A4" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="C4" t="str">
+      <c r="B4" s="24"/>
+      <c r="C4" s="24" t="str">
         <f>C3&amp;C2</f>
         <v>&amp;&lt;&gt;</v>
       </c>
@@ -1986,6 +1998,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -4206,7 +4219,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
new functionality : reading tables
</commit_message>
<xml_diff>
--- a/t/valuereader.xlsx
+++ b/t/valuereader.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Test" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
   </sheets>
   <calcPr calcId="162913"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId6"/>
+    <pivotCache cacheId="1" r:id="rId6"/>
   </pivotCaches>
 </workbook>
 </file>
@@ -1354,7 +1354,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Tableau croisé dynamique2" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valeurs" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Tableau croisé dynamique2" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valeurs" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:E59" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="6">
     <pivotField showAll="0"/>
@@ -1620,13 +1620,7 @@
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Entities" displayName="Entities" ref="A1:F68" totalsRowShown="0">
-  <autoFilter ref="A1:F68">
-    <filterColumn colId="5">
-      <filters>
-        <filter val="cedilla"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:F68"/>
   <tableColumns count="6">
     <tableColumn id="1" name="Num"/>
     <tableColumn id="2" name="Name"/>
@@ -1928,7 +1922,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:C4"/>
     </sheetView>
   </sheetViews>
@@ -2018,8 +2012,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F68"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F44" sqref="F44"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2044,7 +2038,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="2" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>38</v>
       </c>
@@ -2058,7 +2052,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="3" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>62</v>
       </c>
@@ -2072,7 +2066,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>60</v>
       </c>
@@ -2086,7 +2080,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>34</v>
       </c>
@@ -2097,7 +2091,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>39</v>
       </c>
@@ -2111,7 +2105,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>198</v>
       </c>
@@ -2128,7 +2122,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="8" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>193</v>
       </c>
@@ -2148,7 +2142,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="9" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>194</v>
       </c>
@@ -2168,7 +2162,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="10" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>192</v>
       </c>
@@ -2188,7 +2182,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="11" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>197</v>
       </c>
@@ -2208,7 +2202,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="12" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>195</v>
       </c>
@@ -2228,7 +2222,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="13" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>196</v>
       </c>
@@ -2268,7 +2262,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="15" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>208</v>
       </c>
@@ -2288,7 +2282,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="16" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>201</v>
       </c>
@@ -2308,7 +2302,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="17" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>202</v>
       </c>
@@ -2328,7 +2322,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="18" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>200</v>
       </c>
@@ -2348,7 +2342,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="19" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>203</v>
       </c>
@@ -2368,7 +2362,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="20" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>205</v>
       </c>
@@ -2388,7 +2382,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="21" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>206</v>
       </c>
@@ -2408,7 +2402,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="22" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>204</v>
       </c>
@@ -2428,7 +2422,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="23" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>207</v>
       </c>
@@ -2448,7 +2442,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="24" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>209</v>
       </c>
@@ -2468,7 +2462,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="25" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>211</v>
       </c>
@@ -2488,7 +2482,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="26" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>212</v>
       </c>
@@ -2508,7 +2502,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="27" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>210</v>
       </c>
@@ -2528,7 +2522,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="28" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>216</v>
       </c>
@@ -2548,7 +2542,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="29" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>213</v>
       </c>
@@ -2568,7 +2562,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="30" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>214</v>
       </c>
@@ -2588,7 +2582,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="31" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>222</v>
       </c>
@@ -2608,7 +2602,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="32" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>218</v>
       </c>
@@ -2628,7 +2622,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="33" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>219</v>
       </c>
@@ -2648,7 +2642,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="34" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>217</v>
       </c>
@@ -2668,7 +2662,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="35" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>220</v>
       </c>
@@ -2688,7 +2682,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="36" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>221</v>
       </c>
@@ -2708,7 +2702,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="37" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>225</v>
       </c>
@@ -2728,7 +2722,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="38" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>226</v>
       </c>
@@ -2748,7 +2742,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="39" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>230</v>
       </c>
@@ -2765,7 +2759,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="40" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>224</v>
       </c>
@@ -2785,7 +2779,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="41" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>229</v>
       </c>
@@ -2805,7 +2799,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="42" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>227</v>
       </c>
@@ -2825,7 +2819,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="43" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>228</v>
       </c>
@@ -2865,7 +2859,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="45" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>233</v>
       </c>
@@ -2885,7 +2879,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="46" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>234</v>
       </c>
@@ -2905,7 +2899,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="47" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>232</v>
       </c>
@@ -2925,7 +2919,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="48" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>240</v>
       </c>
@@ -2945,7 +2939,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="49" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>235</v>
       </c>
@@ -2965,7 +2959,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="50" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>237</v>
       </c>
@@ -2985,7 +2979,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="51" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>238</v>
       </c>
@@ -3005,7 +2999,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="52" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>236</v>
       </c>
@@ -3025,7 +3019,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="53" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>239</v>
       </c>
@@ -3045,7 +3039,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="54" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>241</v>
       </c>
@@ -3065,7 +3059,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="55" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>243</v>
       </c>
@@ -3085,7 +3079,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="56" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>244</v>
       </c>
@@ -3105,7 +3099,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="57" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>242</v>
       </c>
@@ -3125,7 +3119,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="58" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>248</v>
       </c>
@@ -3145,7 +3139,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="59" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>245</v>
       </c>
@@ -3165,7 +3159,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="60" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>246</v>
       </c>
@@ -3185,7 +3179,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="61" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>223</v>
       </c>
@@ -3205,7 +3199,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="62" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>254</v>
       </c>
@@ -3225,7 +3219,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="63" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>250</v>
       </c>
@@ -3245,7 +3239,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="64" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>251</v>
       </c>
@@ -3265,7 +3259,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="65" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>249</v>
       </c>
@@ -3285,7 +3279,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="66" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>252</v>
       </c>
@@ -3305,7 +3299,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="67" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>253</v>
       </c>
@@ -3325,7 +3319,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="68" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>255</v>
       </c>

</xml_diff>

<commit_message>
tests; support tables in libXML backend
</commit_message>
<xml_diff>
--- a/t/valuereader.xlsx
+++ b/t/valuereader.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Test" sheetId="1" r:id="rId1"/>
@@ -17,16 +17,17 @@
     <sheet name="Entities" sheetId="3" r:id="rId3"/>
     <sheet name="Tab_entities" sheetId="5" r:id="rId4"/>
     <sheet name="Dates" sheetId="6" r:id="rId5"/>
+    <sheet name="Tables" sheetId="7" r:id="rId6"/>
   </sheets>
   <calcPr calcId="162913"/>
   <pivotCaches>
-    <pivotCache cacheId="1" r:id="rId6"/>
+    <pivotCache cacheId="0" r:id="rId7"/>
   </pivotCaches>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="397" uniqueCount="187">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="408" uniqueCount="198">
   <si>
     <t>Hello</t>
   </si>
@@ -612,6 +613,39 @@
     <t>cell
 with
 embedded newlines</t>
+  </si>
+  <si>
+    <t>foo</t>
+  </si>
+  <si>
+    <t>bar</t>
+  </si>
+  <si>
+    <t>badam</t>
+  </si>
+  <si>
+    <t>bum</t>
+  </si>
+  <si>
+    <t>aa</t>
+  </si>
+  <si>
+    <t>bb</t>
+  </si>
+  <si>
+    <t>cc</t>
+  </si>
+  <si>
+    <t>dd</t>
+  </si>
+  <si>
+    <t>ee</t>
+  </si>
+  <si>
+    <t>ff</t>
+  </si>
+  <si>
+    <t>gg</t>
   </si>
 </sst>
 </file>
@@ -1354,7 +1388,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Tableau croisé dynamique2" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valeurs" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Tableau croisé dynamique2" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valeurs" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:E59" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="6">
     <pivotField showAll="0"/>
@@ -1628,6 +1662,39 @@
     <tableColumn id="6" name="Cap/small"/>
     <tableColumn id="4" name="Letter"/>
     <tableColumn id="5" name="Variant"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="tab_foobar" displayName="tab_foobar" ref="A1:B3" totalsRowShown="0">
+  <autoFilter ref="A1:B3"/>
+  <tableColumns count="2">
+    <tableColumn id="1" name="foo"/>
+    <tableColumn id="2" name="bar"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="tab_in_middle_of_sheet" displayName="tab_in_middle_of_sheet" ref="E3:F5" totalsRowShown="0">
+  <autoFilter ref="E3:F5"/>
+  <tableColumns count="2">
+    <tableColumn id="1" name="badam"/>
+    <tableColumn id="2" name="bum"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="tab_without_headers" displayName="tab_without_headers" ref="I2:K4" headerRowCount="0" totalsRowShown="0">
+  <tableColumns count="3">
+    <tableColumn id="1" name="col1"/>
+    <tableColumn id="2" name="col2"/>
+    <tableColumn id="3" name="col3"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2012,7 +2079,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F68"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:F1"/>
     </sheetView>
   </sheetViews>
@@ -4329,4 +4396,91 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I1" sqref="I1:K1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>187</v>
+      </c>
+      <c r="B1" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>11</v>
+      </c>
+      <c r="B2">
+        <v>22</v>
+      </c>
+      <c r="I2" t="s">
+        <v>191</v>
+      </c>
+      <c r="J2" t="s">
+        <v>192</v>
+      </c>
+      <c r="K2" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>33</v>
+      </c>
+      <c r="B3">
+        <v>44</v>
+      </c>
+      <c r="E3" t="s">
+        <v>189</v>
+      </c>
+      <c r="F3" t="s">
+        <v>190</v>
+      </c>
+      <c r="I3" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="E4">
+        <v>99</v>
+      </c>
+      <c r="F4">
+        <v>88</v>
+      </c>
+      <c r="I4" t="s">
+        <v>195</v>
+      </c>
+      <c r="J4" t="s">
+        <v>196</v>
+      </c>
+      <c r="K4" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="E5">
+        <v>77</v>
+      </c>
+      <c r="F5">
+        <v>66</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="3">
+    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
v1.08 support for parsing Excel tables
</commit_message>
<xml_diff>
--- a/t/valuereader.xlsx
+++ b/t/valuereader.xlsx
@@ -21,13 +21,13 @@
   </sheets>
   <calcPr calcId="162913"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId7"/>
+    <pivotCache cacheId="1" r:id="rId7"/>
   </pivotCaches>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="408" uniqueCount="198">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="414" uniqueCount="202">
   <si>
     <t>Hello</t>
   </si>
@@ -646,6 +646,18 @@
   </si>
   <si>
     <t>gg</t>
+  </si>
+  <si>
+    <t>col&lt;</t>
+  </si>
+  <si>
+    <t>col&amp;</t>
+  </si>
+  <si>
+    <t>col&gt;</t>
+  </si>
+  <si>
+    <t>bim</t>
   </si>
 </sst>
 </file>
@@ -1388,7 +1400,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Tableau croisé dynamique2" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valeurs" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Tableau croisé dynamique2" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valeurs" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:E59" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="6">
     <pivotField showAll="0"/>
@@ -1695,6 +1707,18 @@
     <tableColumn id="1" name="col1"/>
     <tableColumn id="2" name="col2"/>
     <tableColumn id="3" name="col3"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Cols_with_entities" displayName="Cols_with_entities" ref="N2:P3" totalsRowShown="0">
+  <autoFilter ref="N2:P3"/>
+  <tableColumns count="3">
+    <tableColumn id="1" name="col&lt;"/>
+    <tableColumn id="2" name="col&amp;"/>
+    <tableColumn id="3" name="col&gt;"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -4400,15 +4424,15 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K5"/>
+  <dimension ref="A1:P5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1:K1"/>
+      <selection activeCell="N2" sqref="N2:P3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>187</v>
       </c>
@@ -4416,7 +4440,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>11</v>
       </c>
@@ -4432,8 +4456,17 @@
       <c r="K2" t="s">
         <v>193</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="N2" t="s">
+        <v>198</v>
+      </c>
+      <c r="O2" t="s">
+        <v>199</v>
+      </c>
+      <c r="P2" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>33</v>
       </c>
@@ -4449,8 +4482,17 @@
       <c r="I3" t="s">
         <v>194</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="N3" t="s">
+        <v>187</v>
+      </c>
+      <c r="O3" t="s">
+        <v>188</v>
+      </c>
+      <c r="P3" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="E4">
         <v>99</v>
       </c>
@@ -4467,7 +4509,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="E5">
         <v>77</v>
       </c>
@@ -4477,10 +4519,11 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="3">
+  <tableParts count="4">
     <tablePart r:id="rId1"/>
     <tablePart r:id="rId2"/>
     <tablePart r:id="rId3"/>
+    <tablePart r:id="rId4"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
iterator methods ivalues and itable
</commit_message>
<xml_diff>
--- a/t/valuereader.xlsx
+++ b/t/valuereader.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
   <workbookPr hidePivotFieldList="1" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git\DAMI\Excel-ValueReader-XLSX\t\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80F5D02D-8160-4731-A45B-1FB9D5529021}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" activeTab="5"/>
+    <workbookView xWindow="30" yWindow="30" windowWidth="28770" windowHeight="16170" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Test" sheetId="1" r:id="rId1"/>
@@ -18,16 +19,30 @@
     <sheet name="Tab_entities" sheetId="5" r:id="rId4"/>
     <sheet name="Dates" sheetId="6" r:id="rId5"/>
     <sheet name="Tables" sheetId="7" r:id="rId6"/>
+    <sheet name="RemoteCells" sheetId="8" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="1" r:id="rId7"/>
+    <pivotCache cacheId="7" r:id="rId8"/>
   </pivotCaches>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="414" uniqueCount="202">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="418" uniqueCount="206">
   <si>
     <t>Hello</t>
   </si>
@@ -659,11 +674,23 @@
   <si>
     <t>bim</t>
   </si>
+  <si>
+    <t>a1</t>
+  </si>
+  <si>
+    <t>b1</t>
+  </si>
+  <si>
+    <t>aaf1</t>
+  </si>
+  <si>
+    <t>a2556</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="13">
     <numFmt numFmtId="164" formatCode="dd/mm/yyyy;@"/>
     <numFmt numFmtId="165" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
@@ -764,7 +791,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="DateStyleddmmyyyy" xfId="1"/>
+    <cellStyle name="DateStyleddmmyyyy" xfId="1" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -781,7 +808,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="Dami Laurent (PJ)" refreshedDate="43983.253371296298" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="67">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Dami Laurent (PJ)" refreshedDate="43983.253371296298" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="67" xr:uid="{00000000-000A-0000-FFFF-FFFF01000000}">
   <cacheSource type="worksheet">
     <worksheetSource name="Entities"/>
   </cacheSource>
@@ -1400,7 +1427,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Tableau croisé dynamique2" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valeurs" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0300-000000000000}" name="Tableau croisé dynamique2" cacheId="7" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valeurs" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:E59" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="6">
     <pivotField showAll="0"/>
@@ -1660,74 +1687,77 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
       <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
     </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
   </extLst>
 </pivotTableDefinition>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Entities" displayName="Entities" ref="A1:F68" totalsRowShown="0">
-  <autoFilter ref="A1:F68"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Entities" displayName="Entities" ref="A1:F68" totalsRowShown="0">
+  <autoFilter ref="A1:F68" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="Num"/>
-    <tableColumn id="2" name="Name"/>
-    <tableColumn id="3" name="Char"/>
-    <tableColumn id="6" name="Cap/small"/>
-    <tableColumn id="4" name="Letter"/>
-    <tableColumn id="5" name="Variant"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Num"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Name"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Char"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Cap/small"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Letter"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Variant"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="tab_foobar" displayName="tab_foobar" ref="A1:B3" totalsRowShown="0">
-  <autoFilter ref="A1:B3"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="tab_foobar" displayName="tab_foobar" ref="A1:B3" totalsRowShown="0">
+  <autoFilter ref="A1:B3" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="2">
-    <tableColumn id="1" name="foo"/>
-    <tableColumn id="2" name="bar"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="foo"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="bar"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="tab_in_middle_of_sheet" displayName="tab_in_middle_of_sheet" ref="E3:F5" totalsRowShown="0">
-  <autoFilter ref="E3:F5"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="tab_in_middle_of_sheet" displayName="tab_in_middle_of_sheet" ref="E3:F5" totalsRowShown="0">
+  <autoFilter ref="E3:F5" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
   <tableColumns count="2">
-    <tableColumn id="1" name="badam"/>
-    <tableColumn id="2" name="bum"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="badam"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="bum"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="tab_without_headers" displayName="tab_without_headers" ref="I2:K4" headerRowCount="0" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="tab_without_headers" displayName="tab_without_headers" ref="I2:K4" headerRowCount="0" totalsRowShown="0">
   <tableColumns count="3">
-    <tableColumn id="1" name="col1"/>
-    <tableColumn id="2" name="col2"/>
-    <tableColumn id="3" name="col3"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="col1"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0300-000002000000}" name="col2"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0300-000003000000}" name="col3"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Cols_with_entities" displayName="Cols_with_entities" ref="N2:P3" totalsRowShown="0">
-  <autoFilter ref="N2:P3"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{00000000-000C-0000-FFFF-FFFF04000000}" name="Cols_with_entities" displayName="Cols_with_entities" ref="N2:P3" totalsRowShown="0">
+  <autoFilter ref="N2:P3" xr:uid="{00000000-0009-0000-0100-000005000000}"/>
   <tableColumns count="3">
-    <tableColumn id="1" name="col&lt;"/>
-    <tableColumn id="2" name="col&amp;"/>
-    <tableColumn id="3" name="col&gt;"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0400-000001000000}" name="col&lt;"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0400-000002000000}" name="col&amp;"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0400-000003000000}" name="col&gt;"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1765,9 +1795,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1802,7 +1832,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1837,7 +1867,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -2010,7 +2040,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2088,7 +2118,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -2100,7 +2130,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:F68"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3439,7 +3469,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A3:E59"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4301,7 +4331,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4423,12 +4453,10 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:P5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N2" sqref="N2:P3"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -4526,4 +4554,33 @@
     <tablePart r:id="rId4"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{582E682E-50E0-4A19-AE29-AB7156837079}">
+  <dimension ref="A1:AAF2556"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:708" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>202</v>
+      </c>
+      <c r="B1" t="s">
+        <v>203</v>
+      </c>
+      <c r="AAF1" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="2556" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2556" t="s">
+        <v>205</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
final tuning for ivalues and itable methods + support for tables with a 'totals' row
</commit_message>
<xml_diff>
--- a/t/valuereader.xlsx
+++ b/t/valuereader.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git\DAMI\Excel-ValueReader-XLSX\t\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80F5D02D-8160-4731-A45B-1FB9D5529021}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37A04D60-D1BF-43D6-A2F9-0BFCEA1BF38B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="30" yWindow="30" windowWidth="28770" windowHeight="16170" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="7" r:id="rId8"/>
+    <pivotCache cacheId="0" r:id="rId8"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="418" uniqueCount="206">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="421" uniqueCount="208">
   <si>
     <t>Hello</t>
   </si>
@@ -685,6 +685,12 @@
   </si>
   <si>
     <t>a2556</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>z</t>
   </si>
 </sst>
 </file>
@@ -1427,7 +1433,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0300-000000000000}" name="Tableau croisé dynamique2" cacheId="7" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valeurs" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0300-000000000000}" name="Tableau croisé dynamique2" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valeurs" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:E59" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="6">
     <pivotField showAll="0"/>
@@ -1749,6 +1755,18 @@
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0400-000001000000}" name="col&lt;"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0400-000002000000}" name="col&amp;"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0400-000003000000}" name="col&gt;"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{5928E664-555F-4F8D-B13C-1C92B6BD1944}" name="HasTotals" displayName="HasTotals" ref="J10:L14" totalsRowCount="1">
+  <autoFilter ref="J10:L13" xr:uid="{5928E664-555F-4F8D-B13C-1C92B6BD1944}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{683EE319-B8C6-4FA4-991D-8789F018628E}" name="x" totalsRowFunction="max"/>
+    <tableColumn id="2" xr3:uid="{14B06313-D92A-4BFB-88CC-7E47FF24B1EF}" name="y" totalsRowFunction="count"/>
+    <tableColumn id="3" xr3:uid="{8C864C05-7D34-42F0-9934-9B2FE0A71400}" name="z" totalsRowFunction="sum"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -4454,9 +4472,11 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:P5"/>
+  <dimension ref="A1:P14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -4545,13 +4565,72 @@
         <v>66</v>
       </c>
     </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="J10" t="s">
+        <v>206</v>
+      </c>
+      <c r="K10" t="s">
+        <v>172</v>
+      </c>
+      <c r="L10" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="J11">
+        <v>11</v>
+      </c>
+      <c r="K11">
+        <v>22</v>
+      </c>
+      <c r="L11">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="J12">
+        <v>44</v>
+      </c>
+      <c r="K12">
+        <v>55</v>
+      </c>
+      <c r="L12">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="J13">
+        <v>77</v>
+      </c>
+      <c r="K13">
+        <v>88</v>
+      </c>
+      <c r="L13">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="J14">
+        <f>SUBTOTAL(104,HasTotals[x])</f>
+        <v>77</v>
+      </c>
+      <c r="K14">
+        <f>SUBTOTAL(103,HasTotals[y])</f>
+        <v>3</v>
+      </c>
+      <c r="L14">
+        <f>SUBTOTAL(109,HasTotals[z])</f>
+        <v>198</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="4">
+  <tableParts count="5">
     <tablePart r:id="rId1"/>
     <tablePart r:id="rId2"/>
     <tablePart r:id="rId3"/>
     <tablePart r:id="rId4"/>
+    <tablePart r:id="rId5"/>
   </tableParts>
 </worksheet>
 </file>

</xml_diff>